<commit_message>
v.2.0.5: Support adjust default value on php style sheet. If specified, double-quotations are added automatially and escape specified double-quotations on String type.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectSample3Structure.xlsx
+++ b/meta/objects/BlancoValueObjectSample3Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObject/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38286C41-EA22-9E4E-AA8B-5B2EE74C4004}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056185BF-CE9B-E943-8298-EF94F7E06AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,14 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="92512" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -291,11 +293,26 @@
   <si>
     <t>public</t>
   </si>
+  <si>
+    <t>field2</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>えおか</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ダブルクォートが付与される</t>
+    <rPh sb="8" eb="10">
+      <t xml:space="preserve">フヨサレル </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -770,6 +787,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -795,9 +815,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1198,13 +1215,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -1280,12 +1299,12 @@
         <v>12</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="46"/>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7">
@@ -1399,24 +1418,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="52"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="48"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="49"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="52"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="48"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="49"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1458,30 +1477,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="49" t="s">
+      <c r="C25" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="49" t="s">
+      <c r="E25" s="50" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1498,18 +1517,29 @@
       <c r="D27" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="46" t="s">
+      <c r="E27" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="47"/>
+      <c r="F27" s="48"/>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="39"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="A28" s="18">
+        <f>A27+1</f>
+        <v>2</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>40</v>
+      </c>
       <c r="F28" s="42"/>
       <c r="G28"/>
     </row>
@@ -1722,38 +1752,38 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D66">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>isAbstract</formula1>
     </dataValidation>
   </dataValidations>
@@ -1766,7 +1796,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>

</xml_diff>